<commit_message>
mudando para registro, checando inscrição e permissao de tabela
</commit_message>
<xml_diff>
--- a/lekopa.xlsx
+++ b/lekopa.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Inscrição</t>
   </si>
@@ -34,13 +34,19 @@
     <t>gutaolox</t>
   </si>
   <si>
-    <t>Mest002</t>
-  </si>
-  <si>
-    <t>Gustavop5</t>
-  </si>
-  <si>
-    <t>GustavoP5</t>
+    <t>Luaniinha23</t>
+  </si>
+  <si>
+    <t>Batman_Bolado</t>
+  </si>
+  <si>
+    <t>Batman Bolado</t>
+  </si>
+  <si>
+    <t>ieko</t>
+  </si>
+  <si>
+    <t>leko</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -351,6 +357,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>